<commit_message>
Add in a table new dish
</commit_message>
<xml_diff>
--- a/Calories dishes.xlsx
+++ b/Calories dishes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\Git\Git\CookingBook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5146CAD-DB8F-4805-BB0D-B2E9341CFA51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23935694-23C8-4DD2-9F32-66B86750DFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C84F12D5-F440-4D32-8BAC-2DB01FD6A34C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Калорийность блюд</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Творог со сметаной</t>
+  </si>
+  <si>
+    <t>Йогурт</t>
   </si>
 </sst>
 </file>
@@ -421,7 +424,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,8 +460,12 @@
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>110</v>
+      </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>